<commit_message>
Corrección de documento de Análisis
</commit_message>
<xml_diff>
--- a/Documentos/Análisis/Selección Múltiple de Clientes en Perfil de Empleados v3.xlsx
+++ b/Documentos/Análisis/Selección Múltiple de Clientes en Perfil de Empleados v3.xlsx
@@ -545,8 +545,8 @@
   </sheetPr>
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>